<commit_message>
xsls - style - more refactoring
</commit_message>
<xml_diff>
--- a/reports/_AJT_SUMMIT ALLIANCE PORT LIMITED_import_container_report_2018-10-08_29_.xlsx
+++ b/reports/_AJT_SUMMIT ALLIANCE PORT LIMITED_import_container_report_2018-10-08_29_.xlsx
@@ -385,12 +385,13 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -543,12 +544,13 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -568,7 +570,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="80.6561797752809" hidden="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="80.6561797752809" hidden="false"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.213483146067416"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="13.213483146067416"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.713483146067416"/>
@@ -689,12 +691,13 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -708,7 +711,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE7"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -776,212 +779,220 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+    <row ht="16" customHeight="true" r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Total number of conatiners:1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Container Number</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D7" s="4" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Agent</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>MLO</t>
         </is>
       </c>
-      <c r="I6" s="4" t="inlineStr">
+      <c r="I7" s="4" t="inlineStr">
         <is>
           <t>Import Vessel</t>
         </is>
       </c>
-      <c r="J6" s="4" t="inlineStr">
+      <c r="J7" s="4" t="inlineStr">
         <is>
           <t>Rotation #</t>
         </is>
       </c>
-      <c r="K6" s="4" t="inlineStr">
+      <c r="K7" s="4" t="inlineStr">
         <is>
           <t>BE #</t>
         </is>
       </c>
-      <c r="L6" s="4" t="inlineStr">
+      <c r="L7" s="4" t="inlineStr">
         <is>
           <t>BL #</t>
         </is>
       </c>
-      <c r="M6" s="4" t="inlineStr">
+      <c r="M7" s="4" t="inlineStr">
         <is>
           <t>Line #</t>
         </is>
       </c>
-      <c r="N6" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr">
         <is>
           <t>Importer</t>
         </is>
       </c>
-      <c r="O6" s="4" t="inlineStr">
+      <c r="O7" s="4" t="inlineStr">
         <is>
           <t>CNF</t>
         </is>
       </c>
-      <c r="P6" s="4" t="inlineStr">
+      <c r="P7" s="4" t="inlineStr">
         <is>
           <t>EIR #</t>
         </is>
       </c>
-      <c r="Q6" s="4" t="inlineStr">
+      <c r="Q7" s="4" t="inlineStr">
         <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="R6" s="4" t="inlineStr">
+      <c r="R7" s="4" t="inlineStr">
         <is>
           <t>Seal Number</t>
         </is>
       </c>
-      <c r="S6" s="4" t="inlineStr">
+      <c r="S7" s="4" t="inlineStr">
         <is>
           <t>Amended Seal No</t>
         </is>
       </c>
-      <c r="T6" s="4" t="inlineStr">
+      <c r="T7" s="4" t="inlineStr">
         <is>
           <t>Location - From</t>
         </is>
       </c>
-      <c r="U6" s="4" t="inlineStr">
+      <c r="U7" s="4" t="inlineStr">
         <is>
           <t>Depo Loc</t>
         </is>
       </c>
-      <c r="V6" s="4" t="inlineStr">
+      <c r="V7" s="4" t="inlineStr">
         <is>
           <t>Issue Date</t>
         </is>
       </c>
-      <c r="W6" s="4" t="inlineStr">
+      <c r="W7" s="4" t="inlineStr">
         <is>
           <t>In Date</t>
         </is>
       </c>
-      <c r="X6" s="4" t="inlineStr">
+      <c r="X7" s="4" t="inlineStr">
         <is>
           <t>Unstuffing Date</t>
         </is>
       </c>
-      <c r="Y6" s="4" t="inlineStr">
+      <c r="Y7" s="4" t="inlineStr">
         <is>
           <t>Container Condition</t>
         </is>
       </c>
-      <c r="Z6" s="4" t="inlineStr">
+      <c r="Z7" s="4" t="inlineStr">
         <is>
           <t>Damage Area</t>
         </is>
       </c>
-      <c r="AA6" s="4" t="inlineStr">
+      <c r="AA7" s="4" t="inlineStr">
         <is>
           <t>Damage Part</t>
         </is>
       </c>
-      <c r="AB6" s="4" t="inlineStr">
+      <c r="AB7" s="4" t="inlineStr">
         <is>
           <t>Damage Description</t>
         </is>
       </c>
-      <c r="AC6" s="4" t="inlineStr">
+      <c r="AC7" s="4" t="inlineStr">
         <is>
           <t>In Transport</t>
         </is>
       </c>
-      <c r="AD6" s="4" t="inlineStr">
+      <c r="AD7" s="4" t="inlineStr">
         <is>
           <t>In Trailer</t>
         </is>
       </c>
-      <c r="AE6" s="4" t="inlineStr">
+      <c r="AE7" s="4" t="inlineStr">
         <is>
           <t>Trailer #</t>
         </is>
       </c>
-      <c r="AF6" s="4" t="inlineStr">
+      <c r="AF7" s="4" t="inlineStr">
         <is>
           <t>In Remarks</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-      <c r="L7" s="0"/>
-      <c r="M7" s="0"/>
-      <c r="N7" s="0"/>
-      <c r="O7" s="0"/>
-      <c r="P7" s="0"/>
-      <c r="Q7" s="0"/>
-      <c r="R7" s="0"/>
-      <c r="S7" s="0"/>
-      <c r="T7" s="0"/>
-      <c r="U7" s="0"/>
-      <c r="V7" s="0"/>
-      <c r="W7" s="0"/>
-      <c r="X7" s="0"/>
-      <c r="Y7" s="0"/>
-      <c r="Z7" s="0"/>
-      <c r="AA7" s="0"/>
-      <c r="AB7" s="0"/>
-      <c r="AC7" s="0"/>
-      <c r="AD7" s="0"/>
-      <c r="AE7" s="0"/>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -1122,12 +1133,13 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -1141,7 +1153,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH7"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1211,215 +1223,223 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+    <row ht="16" customHeight="true" r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Total number of conatiners:1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Container Number</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D7" s="4" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t>Agent</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
         <is>
           <t>MLO</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>Import Vessel</t>
         </is>
       </c>
-      <c r="I6" s="4" t="inlineStr">
+      <c r="I7" s="4" t="inlineStr">
         <is>
           <t>Rotation #</t>
         </is>
       </c>
-      <c r="J6" s="4" t="inlineStr">
+      <c r="J7" s="4" t="inlineStr">
         <is>
           <t>Importer</t>
         </is>
       </c>
-      <c r="K6" s="4" t="inlineStr">
+      <c r="K7" s="4" t="inlineStr">
         <is>
           <t>CNFCommodity</t>
         </is>
       </c>
-      <c r="L6" s="4" t="inlineStr">
+      <c r="L7" s="4" t="inlineStr">
         <is>
           <t>Current Depo</t>
         </is>
       </c>
-      <c r="M6" s="4" t="inlineStr">
+      <c r="M7" s="4" t="inlineStr">
         <is>
           <t>Seal Number</t>
         </is>
       </c>
-      <c r="N6" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr">
         <is>
           <t>Amended Seal No</t>
         </is>
       </c>
-      <c r="O6" s="4" t="inlineStr">
+      <c r="O7" s="4" t="inlineStr">
         <is>
           <t>EIR #</t>
         </is>
       </c>
-      <c r="P6" s="4" t="inlineStr">
+      <c r="P7" s="4" t="inlineStr">
         <is>
           <t>BE #</t>
         </is>
       </c>
-      <c r="Q6" s="4" t="inlineStr">
+      <c r="Q7" s="4" t="inlineStr">
         <is>
           <t>BL #</t>
         </is>
       </c>
-      <c r="R6" s="4" t="inlineStr">
+      <c r="R7" s="4" t="inlineStr">
         <is>
           <t>Line #</t>
         </is>
       </c>
-      <c r="S6" s="4" t="inlineStr">
+      <c r="S7" s="4" t="inlineStr">
         <is>
           <t>Location - From</t>
         </is>
       </c>
-      <c r="T6" s="4" t="inlineStr">
+      <c r="T7" s="4" t="inlineStr">
         <is>
           <t>Depo Loc</t>
         </is>
       </c>
-      <c r="U6" s="4" t="inlineStr">
+      <c r="U7" s="4" t="inlineStr">
         <is>
           <t>Issue Date</t>
         </is>
       </c>
-      <c r="V6" s="4" t="inlineStr">
+      <c r="V7" s="4" t="inlineStr">
         <is>
           <t>In Date</t>
         </is>
       </c>
-      <c r="W6" s="4" t="inlineStr">
+      <c r="W7" s="4" t="inlineStr">
         <is>
           <t>Out Date</t>
         </is>
       </c>
-      <c r="X6" s="4" t="inlineStr">
+      <c r="X7" s="4" t="inlineStr">
         <is>
           <t>Out Location</t>
         </is>
       </c>
-      <c r="Y6" s="4" t="inlineStr">
+      <c r="Y7" s="4" t="inlineStr">
         <is>
           <t>Container Condition</t>
         </is>
       </c>
-      <c r="Z6" s="4" t="inlineStr">
+      <c r="Z7" s="4" t="inlineStr">
         <is>
           <t>Damage Area</t>
         </is>
       </c>
-      <c r="AA6" s="4" t="inlineStr">
+      <c r="AA7" s="4" t="inlineStr">
         <is>
           <t>Damage Part</t>
         </is>
       </c>
-      <c r="AB6" s="4" t="inlineStr">
+      <c r="AB7" s="4" t="inlineStr">
         <is>
           <t>Damage Description</t>
         </is>
       </c>
-      <c r="AC6" s="4" t="inlineStr">
+      <c r="AC7" s="4" t="inlineStr">
         <is>
           <t>Total Lot</t>
         </is>
       </c>
-      <c r="AD6" s="4" t="inlineStr">
+      <c r="AD7" s="4" t="inlineStr">
         <is>
           <t>Total Weight</t>
         </is>
       </c>
-      <c r="AE6" s="4" t="inlineStr">
+      <c r="AE7" s="4" t="inlineStr">
         <is>
           <t>Out Transport</t>
         </is>
       </c>
-      <c r="AF6" s="4" t="inlineStr">
+      <c r="AF7" s="4" t="inlineStr">
         <is>
           <t>Out Remarks</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-      <c r="L7" s="0"/>
-      <c r="M7" s="0"/>
-      <c r="N7" s="0"/>
-      <c r="O7" s="0"/>
-      <c r="P7" s="0"/>
-      <c r="Q7" s="0"/>
-      <c r="R7" s="0"/>
-      <c r="S7" s="0"/>
-      <c r="T7" s="0"/>
-      <c r="U7" s="0"/>
-      <c r="V7" s="0"/>
-      <c r="W7" s="0"/>
-      <c r="X7" s="0"/>
-      <c r="Y7" s="0"/>
-      <c r="Z7" s="0"/>
-      <c r="AA7" s="0"/>
-      <c r="AB7" s="0"/>
-      <c r="AC7" s="0"/>
-      <c r="AD7" s="0"/>
-      <c r="AE7" s="0"/>
-      <c r="AF7" s="0"/>
-      <c r="AG7" s="0"/>
-      <c r="AH7" s="0"/>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="0"/>
+      <c r="AF8" s="0"/>
+      <c r="AG8" s="0"/>
+      <c r="AH8" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -1560,12 +1580,13 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -1579,7 +1600,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1644,195 +1665,203 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+    <row ht="16" customHeight="true" r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Total number of conatiners:1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Container Number</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D7" s="4" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t>Agent</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
         <is>
           <t>MLO</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>Import Vessel</t>
         </is>
       </c>
-      <c r="I6" s="4" t="inlineStr">
+      <c r="I7" s="4" t="inlineStr">
         <is>
           <t>Rotation #</t>
         </is>
       </c>
-      <c r="J6" s="4" t="inlineStr">
+      <c r="J7" s="4" t="inlineStr">
         <is>
           <t>Importer</t>
         </is>
       </c>
-      <c r="K6" s="4" t="inlineStr">
+      <c r="K7" s="4" t="inlineStr">
         <is>
           <t>Container Condition</t>
         </is>
       </c>
-      <c r="L6" s="4" t="inlineStr">
+      <c r="L7" s="4" t="inlineStr">
         <is>
           <t>Damage Area</t>
         </is>
       </c>
-      <c r="M6" s="4" t="inlineStr">
+      <c r="M7" s="4" t="inlineStr">
         <is>
           <t>Damage Part</t>
         </is>
       </c>
-      <c r="N6" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr">
         <is>
           <t>Damage Description</t>
         </is>
       </c>
-      <c r="O6" s="4" t="inlineStr">
+      <c r="O7" s="4" t="inlineStr">
         <is>
           <t>CNF</t>
         </is>
       </c>
-      <c r="P6" s="4" t="inlineStr">
+      <c r="P7" s="4" t="inlineStr">
         <is>
           <t>Commodity</t>
         </is>
       </c>
-      <c r="Q6" s="4" t="inlineStr">
+      <c r="Q7" s="4" t="inlineStr">
         <is>
           <t>Seal Number</t>
         </is>
       </c>
-      <c r="R6" s="4" t="inlineStr">
+      <c r="R7" s="4" t="inlineStr">
         <is>
           <t>Amended Seal No</t>
         </is>
       </c>
-      <c r="S6" s="4" t="inlineStr">
+      <c r="S7" s="4" t="inlineStr">
         <is>
           <t>EIR #</t>
         </is>
       </c>
-      <c r="T6" s="4" t="inlineStr">
+      <c r="T7" s="4" t="inlineStr">
         <is>
           <t>Issue Date</t>
         </is>
       </c>
-      <c r="U6" s="4" t="inlineStr">
+      <c r="U7" s="4" t="inlineStr">
         <is>
           <t>In Date</t>
         </is>
       </c>
-      <c r="V6" s="4" t="inlineStr">
+      <c r="V7" s="4" t="inlineStr">
         <is>
           <t>Location - From</t>
         </is>
       </c>
-      <c r="W6" s="4" t="inlineStr">
+      <c r="W7" s="4" t="inlineStr">
         <is>
           <t>Depo Loc</t>
         </is>
       </c>
-      <c r="X6" s="4" t="inlineStr">
+      <c r="X7" s="4" t="inlineStr">
         <is>
           <t>BE #</t>
         </is>
       </c>
-      <c r="Y6" s="4" t="inlineStr">
+      <c r="Y7" s="4" t="inlineStr">
         <is>
           <t>BL #</t>
         </is>
       </c>
-      <c r="Z6" s="4" t="inlineStr">
+      <c r="Z7" s="4" t="inlineStr">
         <is>
           <t>Line #</t>
         </is>
       </c>
-      <c r="AA6" s="4" t="inlineStr">
+      <c r="AA7" s="4" t="inlineStr">
         <is>
           <t>Trailer #</t>
         </is>
       </c>
-      <c r="AB6" s="4" t="inlineStr">
+      <c r="AB7" s="4" t="inlineStr">
         <is>
           <t>In Transport</t>
         </is>
       </c>
-      <c r="AC6" s="4" t="inlineStr">
+      <c r="AC7" s="4" t="inlineStr">
         <is>
           <t>In Remarks</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="0"/>
-      <c r="K7" s="0"/>
-      <c r="L7" s="0"/>
-      <c r="M7" s="0"/>
-      <c r="N7" s="0"/>
-      <c r="O7" s="0"/>
-      <c r="P7" s="0"/>
-      <c r="Q7" s="0"/>
-      <c r="R7" s="0"/>
-      <c r="S7" s="0"/>
-      <c r="T7" s="0"/>
-      <c r="U7" s="0"/>
-      <c r="V7" s="0"/>
-      <c r="W7" s="0"/>
-      <c r="X7" s="0"/>
-      <c r="Y7" s="0"/>
-      <c r="Z7" s="0"/>
-      <c r="AA7" s="0"/>
-      <c r="AB7" s="0"/>
-      <c r="AC7" s="0"/>
+    <row r="8">
+      <c r="A8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+      <c r="F8" s="0"/>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
+      <c r="O8" s="0"/>
+      <c r="P8" s="0"/>
+      <c r="Q8" s="0"/>
+      <c r="R8" s="0"/>
+      <c r="S8" s="0"/>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+      <c r="V8" s="0"/>
+      <c r="W8" s="0"/>
+      <c r="X8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -1973,12 +2002,13 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
@@ -1992,7 +2022,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -2050,208 +2080,216 @@
         </is>
       </c>
     </row>
-    <row r="5"/>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+    <row ht="16" customHeight="true" r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Total number of conatiners:1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B7" s="4" t="inlineStr">
         <is>
           <t>Container Number</t>
         </is>
       </c>
-      <c r="C6" s="4" t="inlineStr">
+      <c r="C7" s="4" t="inlineStr">
         <is>
           <t>Size</t>
         </is>
       </c>
-      <c r="D6" s="4" t="inlineStr">
+      <c r="D7" s="4" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="E7" s="4" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="F7" s="4" t="inlineStr">
         <is>
           <t>Company</t>
         </is>
       </c>
-      <c r="G6" s="4" t="inlineStr">
+      <c r="G7" s="4" t="inlineStr">
         <is>
           <t>Agent</t>
         </is>
       </c>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="H7" s="4" t="inlineStr">
         <is>
           <t>MLO</t>
         </is>
       </c>
-      <c r="I6" s="4" t="inlineStr">
+      <c r="I7" s="4" t="inlineStr">
         <is>
           <t>Vessel</t>
         </is>
       </c>
-      <c r="J6" s="4" t="inlineStr">
+      <c r="J7" s="4" t="inlineStr">
         <is>
           <t>Rotation #</t>
         </is>
       </c>
-      <c r="K6" s="4" t="inlineStr">
+      <c r="K7" s="4" t="inlineStr">
         <is>
           <t>Line #</t>
         </is>
       </c>
-      <c r="L6" s="4" t="inlineStr">
+      <c r="L7" s="4" t="inlineStr">
         <is>
           <t>BE #</t>
         </is>
       </c>
-      <c r="M6" s="4" t="inlineStr">
+      <c r="M7" s="4" t="inlineStr">
         <is>
           <t>BL #</t>
         </is>
       </c>
-      <c r="N6" s="4" t="inlineStr">
+      <c r="N7" s="4" t="inlineStr">
         <is>
           <t>Importer</t>
         </is>
       </c>
-      <c r="O6" s="4" t="inlineStr">
+      <c r="O7" s="4" t="inlineStr">
         <is>
           <t>CNF</t>
         </is>
       </c>
-      <c r="P6" s="4" t="inlineStr">
+      <c r="P7" s="4" t="inlineStr">
         <is>
           <t>EIR #</t>
         </is>
       </c>
-      <c r="Q6" s="4" t="inlineStr">
+      <c r="Q7" s="4" t="inlineStr">
         <is>
           <t>Location - From</t>
         </is>
       </c>
-      <c r="R6" s="4" t="inlineStr">
+      <c r="R7" s="4" t="inlineStr">
         <is>
           <t>Depo Loc</t>
         </is>
       </c>
-      <c r="S6" s="4" t="inlineStr">
+      <c r="S7" s="4" t="inlineStr">
         <is>
           <t>Seal Number</t>
         </is>
       </c>
-      <c r="T6" s="4" t="inlineStr">
+      <c r="T7" s="4" t="inlineStr">
         <is>
           <t>Amended Seal No</t>
         </is>
       </c>
-      <c r="U6" s="4" t="inlineStr">
+      <c r="U7" s="4" t="inlineStr">
         <is>
           <t>Issue Date</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="n">
+    <row r="8">
+      <c r="A8" s="0" t="n">
         <v>11148</v>
       </c>
-      <c r="B7" s="0" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>CPLU1234560</t>
         </is>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C8" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="D7" s="0" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>GP</t>
         </is>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>8.6</v>
       </c>
-      <c r="F7" s="0" t="inlineStr">
+      <c r="F8" s="0" t="inlineStr">
         <is>
           <t>SAPL-E</t>
         </is>
       </c>
-      <c r="G7" s="0" t="inlineStr">
+      <c r="G8" s="0" t="inlineStr">
         <is>
           <t>AJT</t>
         </is>
       </c>
-      <c r="H7" s="0" t="inlineStr">
+      <c r="H8" s="0" t="inlineStr">
         <is>
           <t>AJT</t>
         </is>
       </c>
-      <c r="I7" s="0" t="inlineStr">
+      <c r="I8" s="0" t="inlineStr">
         <is>
           <t>A IDEFIX</t>
         </is>
       </c>
-      <c r="J7" s="0" t="inlineStr">
+      <c r="J8" s="0" t="inlineStr">
         <is>
           <t>GHHJJHK</t>
         </is>
       </c>
-      <c r="K7" s="0"/>
-      <c r="L7" s="0" t="n">
+      <c r="K8" s="0"/>
+      <c r="L8" s="0" t="n">
         <v>255666</v>
       </c>
-      <c r="M7" s="0"/>
-      <c r="N7" s="0" t="inlineStr">
+      <c r="M8" s="0"/>
+      <c r="N8" s="0" t="inlineStr">
         <is>
           <t>2 C LOGISTICS LTD</t>
         </is>
       </c>
-      <c r="O7" s="0"/>
-      <c r="P7" s="0" t="inlineStr">
+      <c r="O8" s="0"/>
+      <c r="P8" s="0" t="inlineStr">
         <is>
           <t>SAPL/IEIR/2018/11</t>
         </is>
       </c>
-      <c r="Q7" s="0" t="inlineStr">
+      <c r="Q8" s="0" t="inlineStr">
         <is>
           <t>100% COTTON YARN DYED FABRICS</t>
         </is>
       </c>
-      <c r="R7" s="0" t="inlineStr">
+      <c r="R8" s="0" t="inlineStr">
         <is>
           <t>CPA</t>
         </is>
       </c>
-      <c r="S7" s="0" t="inlineStr">
+      <c r="S8" s="0" t="inlineStr">
         <is>
           <t>SAPL</t>
         </is>
       </c>
-      <c r="T7" s="0" t="inlineStr">
+      <c r="T8" s="0" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="U7" s="0"/>
-      <c r="V7" s="0" t="d">
+      <c r="U8" s="0"/>
+      <c r="V8" s="0" t="d">
         <v>2018-10-04T16:47:36.19</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:AD1"/>
     <mergeCell ref="A2:AD2"/>
     <mergeCell ref="A3:AD3"/>
     <mergeCell ref="A4:AD4"/>
     <mergeCell ref="A5:AD5"/>
+    <mergeCell ref="A6:AD6"/>
   </mergeCells>
   <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>

</xml_diff>